<commit_message>
Working code for tracking MB stuff
</commit_message>
<xml_diff>
--- a/MB2016.xlsx
+++ b/MB2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Brian Kim\Code\BKClimbing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umhealth-my.sharepoint.com/personal/kimqi_med_umich_edu/Documents/Desktop/PhD/Code/BKClimbing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85C06CC-E365-49CB-B540-9B53D7394001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{C85C06CC-E365-49CB-B540-9B53D7394001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67911D62-3FF0-4686-BFF1-6642E3FBE33D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="5" xr2:uid="{6F3D7DD2-1A3C-4053-9196-A86ABFA84690}"/>
+    <workbookView xWindow="2136" yWindow="2100" windowWidth="17280" windowHeight="8964" xr2:uid="{6F3D7DD2-1A3C-4053-9196-A86ABFA84690}"/>
   </bookViews>
   <sheets>
     <sheet name="6B+" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="419">
   <si>
     <t>MB ID</t>
   </si>
@@ -1295,6 +1295,9 @@
   </si>
   <si>
     <t>Stoooked</t>
+  </si>
+  <si>
+    <t>Sent</t>
   </si>
 </sst>
 </file>
@@ -1656,19 +1659,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381840D5-B4E3-4353-A910-AA585CF41CA5}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,8 +1684,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1695,8 +1701,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1709,8 +1718,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1723,8 +1735,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1737,8 +1752,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1751,8 +1769,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1765,8 +1786,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1779,8 +1803,11 @@
       <c r="D8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1793,8 +1820,11 @@
       <c r="D9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1807,8 +1837,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1821,8 +1854,11 @@
       <c r="D11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1835,8 +1871,11 @@
       <c r="D12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1849,8 +1888,11 @@
       <c r="D13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1863,8 +1905,11 @@
       <c r="D14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1877,8 +1922,11 @@
       <c r="D15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1892,7 +1940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1906,7 +1954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1920,7 +1968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1934,7 +1982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1948,7 +1996,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1962,7 +2010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1976,7 +2024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1990,7 +2038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2004,7 +2052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2018,7 +2066,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2032,7 +2080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2046,7 +2094,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2060,7 +2108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2074,7 +2122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2088,7 +2136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2102,7 +2150,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2116,7 +2164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2130,7 +2178,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2144,7 +2192,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2158,7 +2206,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2172,7 +2220,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2186,7 +2234,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2200,7 +2248,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2214,7 +2262,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2228,7 +2276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2242,7 +2290,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2256,7 +2304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2270,7 +2318,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2284,7 +2332,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2298,7 +2346,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2312,7 +2360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2326,7 +2374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2340,7 +2388,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2354,7 +2402,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2368,7 +2416,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2382,7 +2430,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2396,7 +2444,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2410,7 +2458,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2424,7 +2472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2438,7 +2486,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2452,7 +2500,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2466,7 +2514,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2480,7 +2528,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2494,7 +2542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2508,7 +2556,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2522,7 +2570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2536,7 +2584,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2550,7 +2598,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2564,7 +2612,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2578,7 +2626,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2592,7 +2640,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2606,7 +2654,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2620,7 +2668,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2634,7 +2682,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2648,7 +2696,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2662,7 +2710,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2676,7 +2724,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2690,7 +2738,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2704,7 +2752,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="2"/>
     </row>
   </sheetData>
@@ -2720,13 +2768,13 @@
       <selection activeCell="A67" sqref="A67:D282"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>74</v>
       </c>
@@ -2754,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>75</v>
       </c>
@@ -2768,7 +2816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>76</v>
       </c>
@@ -2782,7 +2830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>77</v>
       </c>
@@ -2796,7 +2844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>78</v>
       </c>
@@ -2810,7 +2858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>79</v>
       </c>
@@ -2824,7 +2872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80</v>
       </c>
@@ -2838,7 +2886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>81</v>
       </c>
@@ -2852,7 +2900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>82</v>
       </c>
@@ -2866,7 +2914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>83</v>
       </c>
@@ -2880,7 +2928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>84</v>
       </c>
@@ -2894,7 +2942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>85</v>
       </c>
@@ -2908,7 +2956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>86</v>
       </c>
@@ -2922,7 +2970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>87</v>
       </c>
@@ -2936,7 +2984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>88</v>
       </c>
@@ -2950,7 +2998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>89</v>
       </c>
@@ -2964,7 +3012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>90</v>
       </c>
@@ -2978,7 +3026,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>91</v>
       </c>
@@ -2992,7 +3040,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>92</v>
       </c>
@@ -3006,7 +3054,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>93</v>
       </c>
@@ -3020,7 +3068,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>94</v>
       </c>
@@ -3034,7 +3082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>95</v>
       </c>
@@ -3048,7 +3096,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>96</v>
       </c>
@@ -3062,7 +3110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>97</v>
       </c>
@@ -3076,7 +3124,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>98</v>
       </c>
@@ -3090,7 +3138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>99</v>
       </c>
@@ -3104,7 +3152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>100</v>
       </c>
@@ -3118,7 +3166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>101</v>
       </c>
@@ -3132,7 +3180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>102</v>
       </c>
@@ -3146,7 +3194,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>103</v>
       </c>
@@ -3160,7 +3208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>104</v>
       </c>
@@ -3174,7 +3222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>105</v>
       </c>
@@ -3188,7 +3236,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>106</v>
       </c>
@@ -3202,7 +3250,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>107</v>
       </c>
@@ -3216,7 +3264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>108</v>
       </c>
@@ -3230,7 +3278,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>109</v>
       </c>
@@ -3244,7 +3292,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>110</v>
       </c>
@@ -3258,7 +3306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>111</v>
       </c>
@@ -3272,7 +3320,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>112</v>
       </c>
@@ -3286,7 +3334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>113</v>
       </c>
@@ -3300,7 +3348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>114</v>
       </c>
@@ -3314,7 +3362,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>115</v>
       </c>
@@ -3328,7 +3376,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>116</v>
       </c>
@@ -3342,7 +3390,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>117</v>
       </c>
@@ -3356,7 +3404,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>118</v>
       </c>
@@ -3370,7 +3418,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>119</v>
       </c>
@@ -3384,7 +3432,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>120</v>
       </c>
@@ -3398,7 +3446,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>121</v>
       </c>
@@ -3412,7 +3460,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>122</v>
       </c>
@@ -3426,7 +3474,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>123</v>
       </c>
@@ -3440,7 +3488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>124</v>
       </c>
@@ -3454,7 +3502,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>125</v>
       </c>
@@ -3468,7 +3516,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>126</v>
       </c>
@@ -3482,7 +3530,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>127</v>
       </c>
@@ -3496,7 +3544,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>128</v>
       </c>
@@ -3510,7 +3558,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>129</v>
       </c>
@@ -3524,7 +3572,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>130</v>
       </c>
@@ -3538,7 +3586,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>131</v>
       </c>
@@ -3552,7 +3600,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>132</v>
       </c>
@@ -3566,7 +3614,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>133</v>
       </c>
@@ -3580,7 +3628,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>134</v>
       </c>
@@ -3594,7 +3642,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>135</v>
       </c>
@@ -3608,7 +3656,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>136</v>
       </c>
@@ -3622,7 +3670,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>137</v>
       </c>
@@ -3636,7 +3684,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>138</v>
       </c>
@@ -3663,13 +3711,13 @@
       <selection activeCell="A59" sqref="A59:D217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3683,7 +3731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>139</v>
       </c>
@@ -3697,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>140</v>
       </c>
@@ -3711,7 +3759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>141</v>
       </c>
@@ -3725,7 +3773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>142</v>
       </c>
@@ -3739,7 +3787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>143</v>
       </c>
@@ -3753,7 +3801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>144</v>
       </c>
@@ -3767,7 +3815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>145</v>
       </c>
@@ -3781,7 +3829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>146</v>
       </c>
@@ -3795,7 +3843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>147</v>
       </c>
@@ -3809,7 +3857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>148</v>
       </c>
@@ -3823,7 +3871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>149</v>
       </c>
@@ -3837,7 +3885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>150</v>
       </c>
@@ -3851,7 +3899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>151</v>
       </c>
@@ -3865,7 +3913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>152</v>
       </c>
@@ -3879,7 +3927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>153</v>
       </c>
@@ -3893,7 +3941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>154</v>
       </c>
@@ -3907,7 +3955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>155</v>
       </c>
@@ -3921,7 +3969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>156</v>
       </c>
@@ -3935,7 +3983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>157</v>
       </c>
@@ -3949,7 +3997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>158</v>
       </c>
@@ -3963,7 +4011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>159</v>
       </c>
@@ -3977,7 +4025,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>160</v>
       </c>
@@ -3991,7 +4039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>161</v>
       </c>
@@ -4005,7 +4053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>162</v>
       </c>
@@ -4019,7 +4067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>163</v>
       </c>
@@ -4033,7 +4081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>164</v>
       </c>
@@ -4047,7 +4095,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>165</v>
       </c>
@@ -4061,7 +4109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>166</v>
       </c>
@@ -4075,7 +4123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>167</v>
       </c>
@@ -4089,7 +4137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>168</v>
       </c>
@@ -4103,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>169</v>
       </c>
@@ -4117,7 +4165,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>170</v>
       </c>
@@ -4131,7 +4179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>171</v>
       </c>
@@ -4145,7 +4193,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>172</v>
       </c>
@@ -4159,7 +4207,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>173</v>
       </c>
@@ -4173,7 +4221,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>174</v>
       </c>
@@ -4187,7 +4235,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>175</v>
       </c>
@@ -4201,7 +4249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>176</v>
       </c>
@@ -4215,7 +4263,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>177</v>
       </c>
@@ -4229,7 +4277,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>178</v>
       </c>
@@ -4243,7 +4291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>179</v>
       </c>
@@ -4257,7 +4305,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>180</v>
       </c>
@@ -4271,7 +4319,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>181</v>
       </c>
@@ -4285,7 +4333,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>182</v>
       </c>
@@ -4299,7 +4347,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>183</v>
       </c>
@@ -4313,7 +4361,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>184</v>
       </c>
@@ -4327,7 +4375,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>185</v>
       </c>
@@ -4341,7 +4389,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>186</v>
       </c>
@@ -4355,7 +4403,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>187</v>
       </c>
@@ -4369,7 +4417,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>188</v>
       </c>
@@ -4383,7 +4431,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>189</v>
       </c>
@@ -4397,7 +4445,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>190</v>
       </c>
@@ -4411,7 +4459,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>191</v>
       </c>
@@ -4425,7 +4473,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>192</v>
       </c>
@@ -4439,7 +4487,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>193</v>
       </c>
@@ -4453,7 +4501,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>194</v>
       </c>
@@ -4467,7 +4515,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>195</v>
       </c>
@@ -4494,13 +4542,13 @@
       <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4514,7 +4562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>196</v>
       </c>
@@ -4528,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>197</v>
       </c>
@@ -4542,7 +4590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>198</v>
       </c>
@@ -4556,7 +4604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>199</v>
       </c>
@@ -4570,7 +4618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>200</v>
       </c>
@@ -4584,7 +4632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>201</v>
       </c>
@@ -4598,7 +4646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>202</v>
       </c>
@@ -4612,7 +4660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>203</v>
       </c>
@@ -4626,7 +4674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>204</v>
       </c>
@@ -4640,7 +4688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>205</v>
       </c>
@@ -4654,7 +4702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>206</v>
       </c>
@@ -4668,7 +4716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>207</v>
       </c>
@@ -4682,7 +4730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>208</v>
       </c>
@@ -4696,7 +4744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>209</v>
       </c>
@@ -4710,7 +4758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>210</v>
       </c>
@@ -4724,7 +4772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>211</v>
       </c>
@@ -4738,7 +4786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>212</v>
       </c>
@@ -4752,7 +4800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>213</v>
       </c>
@@ -4766,7 +4814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>214</v>
       </c>
@@ -4780,7 +4828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>215</v>
       </c>
@@ -4794,7 +4842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>216</v>
       </c>
@@ -4808,7 +4856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>217</v>
       </c>
@@ -4822,7 +4870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>218</v>
       </c>
@@ -4836,7 +4884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>219</v>
       </c>
@@ -4850,7 +4898,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>220</v>
       </c>
@@ -4864,7 +4912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>221</v>
       </c>
@@ -4878,7 +4926,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>222</v>
       </c>
@@ -4892,7 +4940,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>223</v>
       </c>
@@ -4906,7 +4954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>224</v>
       </c>
@@ -4920,7 +4968,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>225</v>
       </c>
@@ -4934,7 +4982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>226</v>
       </c>
@@ -4948,7 +4996,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>227</v>
       </c>
@@ -4962,7 +5010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>228</v>
       </c>
@@ -4976,7 +5024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>229</v>
       </c>
@@ -4990,7 +5038,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>230</v>
       </c>
@@ -5004,7 +5052,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>231</v>
       </c>
@@ -5018,7 +5066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>232</v>
       </c>
@@ -5032,7 +5080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>233</v>
       </c>
@@ -5046,7 +5094,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>234</v>
       </c>
@@ -5060,7 +5108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>235</v>
       </c>
@@ -5074,7 +5122,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>236</v>
       </c>
@@ -5088,7 +5136,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>237</v>
       </c>
@@ -5102,7 +5150,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>238</v>
       </c>
@@ -5116,7 +5164,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>239</v>
       </c>
@@ -5130,7 +5178,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>240</v>
       </c>
@@ -5144,7 +5192,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>241</v>
       </c>
@@ -5158,7 +5206,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>242</v>
       </c>
@@ -5172,7 +5220,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>243</v>
       </c>
@@ -5186,7 +5234,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>244</v>
       </c>
@@ -5200,7 +5248,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>245</v>
       </c>
@@ -5214,7 +5262,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>246</v>
       </c>
@@ -5228,7 +5276,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>247</v>
       </c>
@@ -5242,7 +5290,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>248</v>
       </c>
@@ -5256,7 +5304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>249</v>
       </c>
@@ -5270,7 +5318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>250</v>
       </c>
@@ -5284,7 +5332,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>251</v>
       </c>
@@ -5298,7 +5346,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>252</v>
       </c>
@@ -5312,7 +5360,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>253</v>
       </c>
@@ -5326,7 +5374,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>254</v>
       </c>
@@ -5340,7 +5388,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>255</v>
       </c>
@@ -5354,7 +5402,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>256</v>
       </c>
@@ -5368,7 +5416,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>257</v>
       </c>
@@ -5382,7 +5430,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>258</v>
       </c>
@@ -5396,7 +5444,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>259</v>
       </c>
@@ -5410,7 +5458,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>260</v>
       </c>
@@ -5424,7 +5472,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>261</v>
       </c>
@@ -5438,7 +5486,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>262</v>
       </c>
@@ -5452,7 +5500,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>263</v>
       </c>
@@ -5466,7 +5514,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>264</v>
       </c>
@@ -5480,7 +5528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>265</v>
       </c>
@@ -5494,7 +5542,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>266</v>
       </c>
@@ -5508,7 +5556,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>267</v>
       </c>
@@ -5522,7 +5570,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>268</v>
       </c>
@@ -5536,7 +5584,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>269</v>
       </c>
@@ -5550,7 +5598,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>270</v>
       </c>
@@ -5564,7 +5612,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>271</v>
       </c>
@@ -5578,7 +5626,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>272</v>
       </c>
@@ -5605,13 +5653,13 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5625,7 +5673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>273</v>
       </c>
@@ -5639,7 +5687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>274</v>
       </c>
@@ -5653,7 +5701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>275</v>
       </c>
@@ -5667,7 +5715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>276</v>
       </c>
@@ -5681,7 +5729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>277</v>
       </c>
@@ -5695,7 +5743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>278</v>
       </c>
@@ -5709,7 +5757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>279</v>
       </c>
@@ -5723,7 +5771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>280</v>
       </c>
@@ -5737,7 +5785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>281</v>
       </c>
@@ -5751,7 +5799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>282</v>
       </c>
@@ -5765,7 +5813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>283</v>
       </c>
@@ -5779,7 +5827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>284</v>
       </c>
@@ -5793,7 +5841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>285</v>
       </c>
@@ -5807,7 +5855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>286</v>
       </c>
@@ -5821,7 +5869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>287</v>
       </c>
@@ -5835,7 +5883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>288</v>
       </c>
@@ -5849,7 +5897,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>289</v>
       </c>
@@ -5863,7 +5911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>290</v>
       </c>
@@ -5877,7 +5925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>291</v>
       </c>
@@ -5891,7 +5939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>292</v>
       </c>
@@ -5905,7 +5953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>293</v>
       </c>
@@ -5919,7 +5967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>294</v>
       </c>
@@ -5933,7 +5981,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>295</v>
       </c>
@@ -5947,7 +5995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>296</v>
       </c>
@@ -5961,7 +6009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>297</v>
       </c>
@@ -5975,7 +6023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>298</v>
       </c>
@@ -5989,7 +6037,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>299</v>
       </c>
@@ -6003,7 +6051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>300</v>
       </c>
@@ -6017,7 +6065,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>301</v>
       </c>
@@ -6031,7 +6079,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>302</v>
       </c>
@@ -6045,7 +6093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>303</v>
       </c>
@@ -6059,7 +6107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>304</v>
       </c>
@@ -6073,7 +6121,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>305</v>
       </c>
@@ -6087,7 +6135,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>306</v>
       </c>
@@ -6101,7 +6149,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>307</v>
       </c>
@@ -6115,7 +6163,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>308</v>
       </c>
@@ -6129,7 +6177,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>309</v>
       </c>
@@ -6143,7 +6191,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>310</v>
       </c>
@@ -6157,7 +6205,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>311</v>
       </c>
@@ -6171,7 +6219,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>312</v>
       </c>
@@ -6185,7 +6233,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>313</v>
       </c>
@@ -6199,7 +6247,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>314</v>
       </c>
@@ -6213,7 +6261,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>315</v>
       </c>
@@ -6227,7 +6275,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>316</v>
       </c>
@@ -6241,7 +6289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>317</v>
       </c>
@@ -6255,7 +6303,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>318</v>
       </c>
@@ -6269,7 +6317,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>319</v>
       </c>
@@ -6283,7 +6331,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>320</v>
       </c>
@@ -6297,7 +6345,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>321</v>
       </c>
@@ -6311,7 +6359,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>322</v>
       </c>
@@ -6325,7 +6373,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>323</v>
       </c>
@@ -6339,7 +6387,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>324</v>
       </c>
@@ -6353,7 +6401,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>325</v>
       </c>
@@ -6367,7 +6415,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>326</v>
       </c>
@@ -6381,7 +6429,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>327</v>
       </c>
@@ -6395,7 +6443,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>328</v>
       </c>
@@ -6409,7 +6457,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>329</v>
       </c>
@@ -6423,7 +6471,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>330</v>
       </c>
@@ -6437,7 +6485,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>331</v>
       </c>
@@ -6451,7 +6499,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>332</v>
       </c>
@@ -6465,7 +6513,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>333</v>
       </c>
@@ -6479,7 +6527,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>334</v>
       </c>
@@ -6493,7 +6541,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>335</v>
       </c>
@@ -6507,7 +6555,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>336</v>
       </c>
@@ -6521,7 +6569,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>337</v>
       </c>
@@ -6535,7 +6583,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>338</v>
       </c>
@@ -6549,7 +6597,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>339</v>
       </c>
@@ -6563,7 +6611,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>340</v>
       </c>
@@ -6577,7 +6625,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>341</v>
       </c>
@@ -6591,7 +6639,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>342</v>
       </c>
@@ -6605,7 +6653,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>343</v>
       </c>
@@ -6619,7 +6667,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>344</v>
       </c>
@@ -6633,7 +6681,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>345</v>
       </c>
@@ -6647,7 +6695,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>346</v>
       </c>
@@ -6661,7 +6709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>347</v>
       </c>
@@ -6675,7 +6723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>348</v>
       </c>
@@ -6689,7 +6737,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>349</v>
       </c>
@@ -6703,7 +6751,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>350</v>
       </c>
@@ -6717,7 +6765,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>351</v>
       </c>
@@ -6731,7 +6779,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>352</v>
       </c>
@@ -6745,7 +6793,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>353</v>
       </c>
@@ -6759,7 +6807,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>354</v>
       </c>
@@ -6780,19 +6828,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B4A294-73D2-4124-9CCD-C57698C1A424}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6805,8 +6853,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>355</v>
       </c>
@@ -6820,7 +6871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>356</v>
       </c>
@@ -6834,7 +6885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>357</v>
       </c>
@@ -6848,7 +6899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>358</v>
       </c>
@@ -6862,7 +6913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>359</v>
       </c>
@@ -6876,7 +6927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>360</v>
       </c>
@@ -6890,7 +6941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>361</v>
       </c>
@@ -6904,7 +6955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>362</v>
       </c>
@@ -6918,7 +6969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>363</v>
       </c>
@@ -6932,7 +6983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>364</v>
       </c>
@@ -6946,7 +6997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>365</v>
       </c>
@@ -6960,7 +7011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>366</v>
       </c>
@@ -6974,7 +7025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>367</v>
       </c>
@@ -6988,7 +7039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>368</v>
       </c>
@@ -7002,7 +7053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>369</v>
       </c>
@@ -7016,7 +7067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>370</v>
       </c>
@@ -7030,7 +7081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>371</v>
       </c>
@@ -7044,7 +7095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>372</v>
       </c>
@@ -7058,7 +7109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>373</v>
       </c>
@@ -7072,7 +7123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>374</v>
       </c>
@@ -7086,7 +7137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>375</v>
       </c>
@@ -7100,7 +7151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>376</v>
       </c>
@@ -7114,7 +7165,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>377</v>
       </c>
@@ -7128,7 +7179,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>378</v>
       </c>
@@ -7142,7 +7193,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>379</v>
       </c>
@@ -7156,7 +7207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>380</v>
       </c>
@@ -7170,7 +7221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>381</v>
       </c>
@@ -7184,7 +7235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>382</v>
       </c>
@@ -7198,7 +7249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>383</v>
       </c>
@@ -7212,7 +7263,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>384</v>
       </c>
@@ -7226,7 +7277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>385</v>
       </c>
@@ -7240,7 +7291,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>386</v>
       </c>
@@ -7254,7 +7305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>387</v>
       </c>
@@ -7268,7 +7319,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>388</v>
       </c>
@@ -7282,7 +7333,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>389</v>
       </c>
@@ -7296,7 +7347,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>390</v>
       </c>
@@ -7310,7 +7361,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>391</v>
       </c>
@@ -7324,7 +7375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>392</v>
       </c>
@@ -7338,7 +7389,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>393</v>
       </c>
@@ -7352,7 +7403,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>394</v>
       </c>
@@ -7366,7 +7417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>395</v>
       </c>
@@ -7380,7 +7431,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>396</v>
       </c>
@@ -7394,7 +7445,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>397</v>
       </c>
@@ -7408,7 +7459,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>398</v>
       </c>
@@ -7422,7 +7473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>399</v>
       </c>
@@ -7436,7 +7487,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>400</v>
       </c>
@@ -7450,7 +7501,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>401</v>
       </c>
@@ -7464,7 +7515,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>402</v>
       </c>
@@ -7478,7 +7529,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>403</v>
       </c>
@@ -7492,7 +7543,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>404</v>
       </c>
@@ -7506,7 +7557,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>405</v>
       </c>
@@ -7520,7 +7571,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>406</v>
       </c>
@@ -7534,7 +7585,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>407</v>
       </c>
@@ -7548,7 +7599,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>408</v>
       </c>
@@ -7562,7 +7613,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>409</v>
       </c>
@@ -7576,7 +7627,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>410</v>
       </c>
@@ -7590,7 +7641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>411</v>
       </c>
@@ -7604,7 +7655,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>412</v>
       </c>
@@ -7618,7 +7669,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>413</v>
       </c>
@@ -7632,7 +7683,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>414</v>
       </c>

</xml_diff>

<commit_message>
New Load Prediction Script
</commit_message>
<xml_diff>
--- a/MB2016.xlsx
+++ b/MB2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umhealth-my.sharepoint.com/personal/kimqi_med_umich_edu/Documents/Desktop/PhD/Code/BKClimbing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Brian Kim\Code\BKClimbing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{C85C06CC-E365-49CB-B540-9B53D7394001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67911D62-3FF0-4686-BFF1-6642E3FBE33D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623B10D6-CC49-4365-BCC4-FE120E3B609D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2136" yWindow="2100" windowWidth="17280" windowHeight="8964" xr2:uid="{6F3D7DD2-1A3C-4053-9196-A86ABFA84690}"/>
+    <workbookView xWindow="5700" yWindow="2910" windowWidth="30375" windowHeight="16905" activeTab="1" xr2:uid="{6F3D7DD2-1A3C-4053-9196-A86ABFA84690}"/>
   </bookViews>
   <sheets>
     <sheet name="6B+" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="419">
   <si>
     <t>MB ID</t>
   </si>
@@ -1661,17 +1661,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381840D5-B4E3-4353-A910-AA585CF41CA5}">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1939,8 +1939,11 @@
       <c r="D16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1953,8 +1956,11 @@
       <c r="D17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1967,8 +1973,11 @@
       <c r="D18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1981,8 +1990,11 @@
       <c r="D19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1995,8 +2007,11 @@
       <c r="D20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2009,8 +2024,11 @@
       <c r="D21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2023,8 +2041,11 @@
       <c r="D22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2037,8 +2058,11 @@
       <c r="D23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2051,8 +2075,11 @@
       <c r="D24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2065,8 +2092,11 @@
       <c r="D25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2079,8 +2109,11 @@
       <c r="D26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2093,8 +2126,11 @@
       <c r="D27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2107,8 +2143,11 @@
       <c r="D28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2121,8 +2160,11 @@
       <c r="D29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2135,8 +2177,11 @@
       <c r="D30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2149,8 +2194,11 @@
       <c r="D31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2163,8 +2211,11 @@
       <c r="D32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2177,8 +2228,11 @@
       <c r="D33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2191,8 +2245,11 @@
       <c r="D34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2205,8 +2262,11 @@
       <c r="D35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2219,8 +2279,11 @@
       <c r="D36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2233,8 +2296,11 @@
       <c r="D37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2247,8 +2313,11 @@
       <c r="D38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2261,8 +2330,11 @@
       <c r="D39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2275,8 +2347,11 @@
       <c r="D40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2290,7 +2365,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2303,8 +2378,11 @@
       <c r="D42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2317,8 +2395,11 @@
       <c r="D43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2332,7 +2413,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2346,7 +2427,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2360,7 +2441,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2373,8 +2454,11 @@
       <c r="D47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2388,7 +2472,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2401,8 +2485,11 @@
       <c r="D49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2416,7 +2503,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2430,7 +2517,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2444,7 +2531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2458,7 +2545,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2471,8 +2558,11 @@
       <c r="D54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2486,7 +2576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2500,7 +2590,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2514,7 +2604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2527,8 +2617,11 @@
       <c r="D58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2542,7 +2635,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2555,8 +2648,11 @@
       <c r="D60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2569,8 +2665,11 @@
       <c r="D61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2584,7 +2683,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2597,8 +2696,11 @@
       <c r="D63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2612,7 +2714,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2626,7 +2728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2640,7 +2742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2653,8 +2755,11 @@
       <c r="D67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2668,7 +2773,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2682,7 +2787,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2695,8 +2800,11 @@
       <c r="D70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2709,8 +2817,11 @@
       <c r="D71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2723,8 +2834,11 @@
       <c r="D72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2737,8 +2851,11 @@
       <c r="D73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2751,8 +2868,11 @@
       <c r="D74">
         <v>73</v>
       </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" s="2"/>
     </row>
   </sheetData>
@@ -2762,19 +2882,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656CECD5-4C49-445E-BBAC-D07773EFADFF}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:D282"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2787,8 +2907,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>74</v>
       </c>
@@ -2801,8 +2924,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>75</v>
       </c>
@@ -2815,8 +2941,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>76</v>
       </c>
@@ -2829,8 +2958,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>77</v>
       </c>
@@ -2843,8 +2975,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>78</v>
       </c>
@@ -2857,8 +2992,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>79</v>
       </c>
@@ -2871,8 +3009,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>80</v>
       </c>
@@ -2885,8 +3026,11 @@
       <c r="D8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>81</v>
       </c>
@@ -2899,8 +3043,11 @@
       <c r="D9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>82</v>
       </c>
@@ -2913,8 +3060,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>83</v>
       </c>
@@ -2927,8 +3077,11 @@
       <c r="D11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>84</v>
       </c>
@@ -2941,8 +3094,11 @@
       <c r="D12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>85</v>
       </c>
@@ -2955,8 +3111,11 @@
       <c r="D13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>86</v>
       </c>
@@ -2970,7 +3129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>87</v>
       </c>
@@ -2984,7 +3143,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88</v>
       </c>
@@ -2998,7 +3157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89</v>
       </c>
@@ -3011,8 +3170,11 @@
       <c r="D17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>90</v>
       </c>
@@ -3025,8 +3187,11 @@
       <c r="D18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>91</v>
       </c>
@@ -3039,8 +3204,11 @@
       <c r="D19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>92</v>
       </c>
@@ -3054,7 +3222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>93</v>
       </c>
@@ -3068,7 +3236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>94</v>
       </c>
@@ -3082,7 +3250,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>95</v>
       </c>
@@ -3096,7 +3264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>96</v>
       </c>
@@ -3110,7 +3278,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>97</v>
       </c>
@@ -3124,7 +3292,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>98</v>
       </c>
@@ -3137,8 +3305,11 @@
       <c r="D26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>99</v>
       </c>
@@ -3152,7 +3323,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>100</v>
       </c>
@@ -3166,7 +3337,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>101</v>
       </c>
@@ -3179,8 +3350,11 @@
       <c r="D29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>102</v>
       </c>
@@ -3194,7 +3368,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>103</v>
       </c>
@@ -3208,7 +3382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>104</v>
       </c>
@@ -3221,8 +3395,11 @@
       <c r="D32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>105</v>
       </c>
@@ -3235,8 +3412,11 @@
       <c r="D33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>106</v>
       </c>
@@ -3250,7 +3430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>107</v>
       </c>
@@ -3264,7 +3444,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>108</v>
       </c>
@@ -3277,8 +3457,11 @@
       <c r="D36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>109</v>
       </c>
@@ -3291,8 +3474,11 @@
       <c r="D37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>110</v>
       </c>
@@ -3306,7 +3492,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>111</v>
       </c>
@@ -3319,8 +3505,11 @@
       <c r="D39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>112</v>
       </c>
@@ -3333,8 +3522,11 @@
       <c r="D40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>113</v>
       </c>
@@ -3348,7 +3540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>114</v>
       </c>
@@ -3362,7 +3554,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>115</v>
       </c>
@@ -3376,7 +3568,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>116</v>
       </c>
@@ -3390,7 +3582,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>117</v>
       </c>
@@ -3403,8 +3595,11 @@
       <c r="D45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>118</v>
       </c>
@@ -3418,7 +3613,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>119</v>
       </c>
@@ -3431,8 +3626,11 @@
       <c r="D47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>120</v>
       </c>
@@ -3446,7 +3644,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>121</v>
       </c>
@@ -3460,7 +3658,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>122</v>
       </c>
@@ -3473,8 +3671,11 @@
       <c r="D50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>123</v>
       </c>
@@ -3487,8 +3688,11 @@
       <c r="D51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>124</v>
       </c>
@@ -3502,7 +3706,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>125</v>
       </c>
@@ -3516,7 +3720,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>126</v>
       </c>
@@ -3530,7 +3734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>127</v>
       </c>
@@ -3543,8 +3747,11 @@
       <c r="D55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>128</v>
       </c>
@@ -3557,8 +3764,11 @@
       <c r="D56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>129</v>
       </c>
@@ -3572,7 +3782,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>130</v>
       </c>
@@ -3586,7 +3796,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>131</v>
       </c>
@@ -3599,8 +3809,11 @@
       <c r="D59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>132</v>
       </c>
@@ -3614,7 +3827,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>133</v>
       </c>
@@ -3627,8 +3840,11 @@
       <c r="D61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>134</v>
       </c>
@@ -3642,7 +3858,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>135</v>
       </c>
@@ -3655,8 +3871,11 @@
       <c r="D63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>136</v>
       </c>
@@ -3669,8 +3888,11 @@
       <c r="D64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>137</v>
       </c>
@@ -3684,7 +3906,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>138</v>
       </c>
@@ -3696,6 +3918,9 @@
       </c>
       <c r="D66">
         <v>65</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3705,19 +3930,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38483A4F-EF33-48B5-88FE-5D5B0B049136}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:D217"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3730,8 +3955,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>139</v>
       </c>
@@ -3744,8 +3972,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>140</v>
       </c>
@@ -3758,8 +3989,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>141</v>
       </c>
@@ -3772,8 +4006,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>142</v>
       </c>
@@ -3786,8 +4023,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>143</v>
       </c>
@@ -3800,8 +4040,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>144</v>
       </c>
@@ -3814,8 +4057,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>145</v>
       </c>
@@ -3828,8 +4074,11 @@
       <c r="D8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>146</v>
       </c>
@@ -3842,8 +4091,11 @@
       <c r="D9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>147</v>
       </c>
@@ -3856,8 +4108,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>148</v>
       </c>
@@ -3870,8 +4125,11 @@
       <c r="D11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>149</v>
       </c>
@@ -3884,8 +4142,11 @@
       <c r="D12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>150</v>
       </c>
@@ -3898,8 +4159,11 @@
       <c r="D13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>151</v>
       </c>
@@ -3912,8 +4176,11 @@
       <c r="D14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>152</v>
       </c>
@@ -3927,7 +4194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>153</v>
       </c>
@@ -3940,8 +4207,11 @@
       <c r="D16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>154</v>
       </c>
@@ -3955,7 +4225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>155</v>
       </c>
@@ -3969,7 +4239,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>156</v>
       </c>
@@ -3983,7 +4253,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>157</v>
       </c>
@@ -3996,8 +4266,11 @@
       <c r="D20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>158</v>
       </c>
@@ -4011,7 +4284,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>159</v>
       </c>
@@ -4025,7 +4298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>160</v>
       </c>
@@ -4038,8 +4311,11 @@
       <c r="D23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>161</v>
       </c>
@@ -4053,7 +4329,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>162</v>
       </c>
@@ -4067,7 +4343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>163</v>
       </c>
@@ -4081,7 +4357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>164</v>
       </c>
@@ -4095,7 +4371,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>165</v>
       </c>
@@ -4108,8 +4384,11 @@
       <c r="D28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>166</v>
       </c>
@@ -4123,7 +4402,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>167</v>
       </c>
@@ -4136,8 +4415,11 @@
       <c r="D30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>168</v>
       </c>
@@ -4151,7 +4433,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>169</v>
       </c>
@@ -4165,7 +4447,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>170</v>
       </c>
@@ -4178,8 +4460,11 @@
       <c r="D33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>171</v>
       </c>
@@ -4193,7 +4478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>172</v>
       </c>
@@ -4207,7 +4492,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>173</v>
       </c>
@@ -4221,7 +4506,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>174</v>
       </c>
@@ -4235,7 +4520,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>175</v>
       </c>
@@ -4248,8 +4533,11 @@
       <c r="D38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>176</v>
       </c>
@@ -4262,8 +4550,11 @@
       <c r="D39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>177</v>
       </c>
@@ -4277,7 +4568,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>178</v>
       </c>
@@ -4291,7 +4582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>179</v>
       </c>
@@ -4305,7 +4596,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>180</v>
       </c>
@@ -4318,8 +4609,11 @@
       <c r="D43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>181</v>
       </c>
@@ -4332,8 +4626,11 @@
       <c r="D44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>182</v>
       </c>
@@ -4347,7 +4644,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>183</v>
       </c>
@@ -4361,7 +4658,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>184</v>
       </c>
@@ -4375,7 +4672,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>185</v>
       </c>
@@ -4389,7 +4686,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>186</v>
       </c>
@@ -4402,8 +4699,11 @@
       <c r="D49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>187</v>
       </c>
@@ -4416,8 +4716,11 @@
       <c r="D50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>188</v>
       </c>
@@ -4431,7 +4734,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>189</v>
       </c>
@@ -4445,7 +4748,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>190</v>
       </c>
@@ -4459,7 +4762,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>191</v>
       </c>
@@ -4473,7 +4776,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>192</v>
       </c>
@@ -4487,7 +4790,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>193</v>
       </c>
@@ -4500,8 +4803,11 @@
       <c r="D56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>194</v>
       </c>
@@ -4514,8 +4820,11 @@
       <c r="D57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>195</v>
       </c>
@@ -4536,19 +4845,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD24673-6124-46AC-8216-9F510582E2DF}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4561,8 +4870,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>196</v>
       </c>
@@ -4576,7 +4888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>197</v>
       </c>
@@ -4590,7 +4902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>198</v>
       </c>
@@ -4604,7 +4916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>199</v>
       </c>
@@ -4618,7 +4930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -4632,7 +4944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>201</v>
       </c>
@@ -4646,7 +4958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>202</v>
       </c>
@@ -4660,7 +4972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>203</v>
       </c>
@@ -4674,7 +4986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>204</v>
       </c>
@@ -4688,7 +5000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>205</v>
       </c>
@@ -4702,7 +5014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>206</v>
       </c>
@@ -4716,7 +5028,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>207</v>
       </c>
@@ -4730,7 +5042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>208</v>
       </c>
@@ -4744,7 +5056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>209</v>
       </c>
@@ -4758,7 +5070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>210</v>
       </c>
@@ -4772,7 +5084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>211</v>
       </c>
@@ -4786,7 +5098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>212</v>
       </c>
@@ -4800,7 +5112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>213</v>
       </c>
@@ -4814,7 +5126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>214</v>
       </c>
@@ -4828,7 +5140,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>215</v>
       </c>
@@ -4842,7 +5154,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>216</v>
       </c>
@@ -4856,7 +5168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>217</v>
       </c>
@@ -4870,7 +5182,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>218</v>
       </c>
@@ -4884,7 +5196,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>219</v>
       </c>
@@ -4898,7 +5210,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>220</v>
       </c>
@@ -4912,7 +5224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>221</v>
       </c>
@@ -4926,7 +5238,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>222</v>
       </c>
@@ -4940,7 +5252,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>223</v>
       </c>
@@ -4954,7 +5266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>224</v>
       </c>
@@ -4968,7 +5280,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>225</v>
       </c>
@@ -4982,7 +5294,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>226</v>
       </c>
@@ -4996,7 +5308,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>227</v>
       </c>
@@ -5010,7 +5322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>228</v>
       </c>
@@ -5024,7 +5336,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>229</v>
       </c>
@@ -5038,7 +5350,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>230</v>
       </c>
@@ -5052,7 +5364,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>231</v>
       </c>
@@ -5066,7 +5378,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>232</v>
       </c>
@@ -5080,7 +5392,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>233</v>
       </c>
@@ -5094,7 +5406,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>234</v>
       </c>
@@ -5108,7 +5420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>235</v>
       </c>
@@ -5122,7 +5434,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>236</v>
       </c>
@@ -5136,7 +5448,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>237</v>
       </c>
@@ -5150,7 +5462,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>238</v>
       </c>
@@ -5164,7 +5476,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>239</v>
       </c>
@@ -5178,7 +5490,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>240</v>
       </c>
@@ -5192,7 +5504,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>241</v>
       </c>
@@ -5206,7 +5518,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>242</v>
       </c>
@@ -5220,7 +5532,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>243</v>
       </c>
@@ -5234,7 +5546,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>244</v>
       </c>
@@ -5248,7 +5560,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>245</v>
       </c>
@@ -5262,7 +5574,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>246</v>
       </c>
@@ -5276,7 +5588,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>247</v>
       </c>
@@ -5290,7 +5602,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>248</v>
       </c>
@@ -5304,7 +5616,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>249</v>
       </c>
@@ -5318,7 +5630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>250</v>
       </c>
@@ -5332,7 +5644,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>251</v>
       </c>
@@ -5346,7 +5658,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>252</v>
       </c>
@@ -5360,7 +5672,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>253</v>
       </c>
@@ -5374,7 +5686,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>254</v>
       </c>
@@ -5388,7 +5700,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>255</v>
       </c>
@@ -5402,7 +5714,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>256</v>
       </c>
@@ -5416,7 +5728,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>257</v>
       </c>
@@ -5430,7 +5742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>258</v>
       </c>
@@ -5444,7 +5756,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>259</v>
       </c>
@@ -5458,7 +5770,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>260</v>
       </c>
@@ -5472,7 +5784,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>261</v>
       </c>
@@ -5486,7 +5798,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>262</v>
       </c>
@@ -5500,7 +5812,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>263</v>
       </c>
@@ -5514,7 +5826,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>264</v>
       </c>
@@ -5528,7 +5840,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>265</v>
       </c>
@@ -5542,7 +5854,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>266</v>
       </c>
@@ -5556,7 +5868,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>267</v>
       </c>
@@ -5570,7 +5882,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>268</v>
       </c>
@@ -5584,7 +5896,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>269</v>
       </c>
@@ -5598,7 +5910,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>270</v>
       </c>
@@ -5612,7 +5924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>271</v>
       </c>
@@ -5626,7 +5938,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>272</v>
       </c>
@@ -5647,19 +5959,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D66F591-3313-4F55-AE9E-961B94EB7958}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5672,8 +5984,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>273</v>
       </c>
@@ -5687,7 +6002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>274</v>
       </c>
@@ -5701,7 +6016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>275</v>
       </c>
@@ -5715,7 +6030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>276</v>
       </c>
@@ -5729,7 +6044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>277</v>
       </c>
@@ -5743,7 +6058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>278</v>
       </c>
@@ -5757,7 +6072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>279</v>
       </c>
@@ -5771,7 +6086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>280</v>
       </c>
@@ -5785,7 +6100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>281</v>
       </c>
@@ -5799,7 +6114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>282</v>
       </c>
@@ -5813,7 +6128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>283</v>
       </c>
@@ -5827,7 +6142,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>284</v>
       </c>
@@ -5841,7 +6156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>285</v>
       </c>
@@ -5855,7 +6170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>286</v>
       </c>
@@ -5869,7 +6184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>287</v>
       </c>
@@ -5883,7 +6198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>288</v>
       </c>
@@ -5897,7 +6212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>289</v>
       </c>
@@ -5911,7 +6226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>290</v>
       </c>
@@ -5925,7 +6240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>291</v>
       </c>
@@ -5939,7 +6254,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>292</v>
       </c>
@@ -5953,7 +6268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>293</v>
       </c>
@@ -5967,7 +6282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>294</v>
       </c>
@@ -5981,7 +6296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>295</v>
       </c>
@@ -5995,7 +6310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>296</v>
       </c>
@@ -6009,7 +6324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>297</v>
       </c>
@@ -6023,7 +6338,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>298</v>
       </c>
@@ -6037,7 +6352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>299</v>
       </c>
@@ -6051,7 +6366,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>300</v>
       </c>
@@ -6065,7 +6380,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>301</v>
       </c>
@@ -6079,7 +6394,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>302</v>
       </c>
@@ -6093,7 +6408,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>303</v>
       </c>
@@ -6107,7 +6422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>304</v>
       </c>
@@ -6121,7 +6436,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>305</v>
       </c>
@@ -6135,7 +6450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>306</v>
       </c>
@@ -6149,7 +6464,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>307</v>
       </c>
@@ -6163,7 +6478,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>308</v>
       </c>
@@ -6177,7 +6492,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>309</v>
       </c>
@@ -6191,7 +6506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>310</v>
       </c>
@@ -6205,7 +6520,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>311</v>
       </c>
@@ -6219,7 +6534,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>312</v>
       </c>
@@ -6233,7 +6548,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>313</v>
       </c>
@@ -6247,7 +6562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>314</v>
       </c>
@@ -6261,7 +6576,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>315</v>
       </c>
@@ -6275,7 +6590,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>316</v>
       </c>
@@ -6289,7 +6604,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>317</v>
       </c>
@@ -6303,7 +6618,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>318</v>
       </c>
@@ -6317,7 +6632,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>319</v>
       </c>
@@ -6331,7 +6646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>320</v>
       </c>
@@ -6345,7 +6660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>321</v>
       </c>
@@ -6359,7 +6674,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>322</v>
       </c>
@@ -6373,7 +6688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>323</v>
       </c>
@@ -6387,7 +6702,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>324</v>
       </c>
@@ -6401,7 +6716,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>325</v>
       </c>
@@ -6415,7 +6730,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>326</v>
       </c>
@@ -6429,7 +6744,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>327</v>
       </c>
@@ -6443,7 +6758,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>328</v>
       </c>
@@ -6457,7 +6772,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>329</v>
       </c>
@@ -6471,7 +6786,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>330</v>
       </c>
@@ -6485,7 +6800,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>331</v>
       </c>
@@ -6499,7 +6814,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>332</v>
       </c>
@@ -6513,7 +6828,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>333</v>
       </c>
@@ -6527,7 +6842,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>334</v>
       </c>
@@ -6541,7 +6856,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>335</v>
       </c>
@@ -6555,7 +6870,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>336</v>
       </c>
@@ -6569,7 +6884,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>337</v>
       </c>
@@ -6583,7 +6898,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>338</v>
       </c>
@@ -6597,7 +6912,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>339</v>
       </c>
@@ -6611,7 +6926,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>340</v>
       </c>
@@ -6625,7 +6940,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>341</v>
       </c>
@@ -6639,7 +6954,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>342</v>
       </c>
@@ -6653,7 +6968,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>343</v>
       </c>
@@ -6667,7 +6982,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>344</v>
       </c>
@@ -6681,7 +6996,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>345</v>
       </c>
@@ -6695,7 +7010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>346</v>
       </c>
@@ -6709,7 +7024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>347</v>
       </c>
@@ -6723,7 +7038,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>348</v>
       </c>
@@ -6737,7 +7052,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>349</v>
       </c>
@@ -6751,7 +7066,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>350</v>
       </c>
@@ -6765,7 +7080,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>351</v>
       </c>
@@ -6779,7 +7094,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>352</v>
       </c>
@@ -6793,7 +7108,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>353</v>
       </c>
@@ -6807,7 +7122,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>354</v>
       </c>
@@ -6831,16 +7146,16 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6857,7 +7172,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>355</v>
       </c>
@@ -6871,7 +7186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>356</v>
       </c>
@@ -6885,7 +7200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>357</v>
       </c>
@@ -6899,7 +7214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>358</v>
       </c>
@@ -6913,7 +7228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>359</v>
       </c>
@@ -6927,7 +7242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>360</v>
       </c>
@@ -6941,7 +7256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>361</v>
       </c>
@@ -6955,7 +7270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>362</v>
       </c>
@@ -6969,7 +7284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>363</v>
       </c>
@@ -6983,7 +7298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>364</v>
       </c>
@@ -6997,7 +7312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>365</v>
       </c>
@@ -7011,7 +7326,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>366</v>
       </c>
@@ -7025,7 +7340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>367</v>
       </c>
@@ -7039,7 +7354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>368</v>
       </c>
@@ -7053,7 +7368,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>369</v>
       </c>
@@ -7067,7 +7382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>370</v>
       </c>
@@ -7081,7 +7396,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>371</v>
       </c>
@@ -7095,7 +7410,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>372</v>
       </c>
@@ -7109,7 +7424,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>373</v>
       </c>
@@ -7123,7 +7438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>374</v>
       </c>
@@ -7137,7 +7452,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>375</v>
       </c>
@@ -7151,7 +7466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>376</v>
       </c>
@@ -7165,7 +7480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>377</v>
       </c>
@@ -7179,7 +7494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>378</v>
       </c>
@@ -7193,7 +7508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>379</v>
       </c>
@@ -7207,7 +7522,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>380</v>
       </c>
@@ -7221,7 +7536,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>381</v>
       </c>
@@ -7235,7 +7550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>382</v>
       </c>
@@ -7249,7 +7564,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>383</v>
       </c>
@@ -7263,7 +7578,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>384</v>
       </c>
@@ -7277,7 +7592,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>385</v>
       </c>
@@ -7291,7 +7606,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>386</v>
       </c>
@@ -7305,7 +7620,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>387</v>
       </c>
@@ -7319,7 +7634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>388</v>
       </c>
@@ -7333,7 +7648,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>389</v>
       </c>
@@ -7347,7 +7662,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>390</v>
       </c>
@@ -7361,7 +7676,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>391</v>
       </c>
@@ -7375,7 +7690,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>392</v>
       </c>
@@ -7389,7 +7704,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>393</v>
       </c>
@@ -7403,7 +7718,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>394</v>
       </c>
@@ -7417,7 +7732,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>395</v>
       </c>
@@ -7431,7 +7746,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>396</v>
       </c>
@@ -7445,7 +7760,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>397</v>
       </c>
@@ -7459,7 +7774,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>398</v>
       </c>
@@ -7473,7 +7788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>399</v>
       </c>
@@ -7487,7 +7802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>400</v>
       </c>
@@ -7501,7 +7816,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>401</v>
       </c>
@@ -7515,7 +7830,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>402</v>
       </c>
@@ -7529,7 +7844,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>403</v>
       </c>
@@ -7543,7 +7858,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>404</v>
       </c>
@@ -7557,7 +7872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>405</v>
       </c>
@@ -7571,7 +7886,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>406</v>
       </c>
@@ -7585,7 +7900,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>407</v>
       </c>
@@ -7599,7 +7914,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>408</v>
       </c>
@@ -7613,7 +7928,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>409</v>
       </c>
@@ -7627,7 +7942,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>410</v>
       </c>
@@ -7641,7 +7956,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>411</v>
       </c>
@@ -7655,7 +7970,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>412</v>
       </c>
@@ -7669,7 +7984,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>413</v>
       </c>
@@ -7683,7 +7998,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>414</v>
       </c>

</xml_diff>